<commit_message>
data updates for co2 and non-co2 ghgs
</commit_message>
<xml_diff>
--- a/data-extra/ghgi/compiled_tables.xlsx
+++ b/data-extra/ghgi/compiled_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-extra\ghgi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBB6E6C-CF8D-42BA-90F3-28101529A6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB6F45F-6074-4792-B4A9-0A9EAC755F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11595" yWindow="4830" windowWidth="17310" windowHeight="9045" tabRatio="825" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="913" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ES-2" sheetId="8" r:id="rId1"/>
@@ -1965,10 +1965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39DF301-64CD-45E3-A2E1-AE655CCC02E7}">
-  <dimension ref="A1:AG21"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3496,30 +3496,33 @@
         <v>5586</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37539,10 +37542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFE04F3-B00A-4F8E-BE69-EC8426234705}">
-  <dimension ref="A1:AH14"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38382,6 +38385,12 @@
       <c r="B14" t="s">
         <v>112</v>
       </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -54094,7 +54103,7 @@
   <dimension ref="A1:AH15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B4" sqref="B4:AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67782,8 +67791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E8144B-1C11-4177-8245-7038D2F2052C}">
   <dimension ref="A1:BQ111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78066,9 +78075,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D979E9A9-3B42-4B36-9C36-335F1BD3B124}">
   <dimension ref="A1:AI72"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -84386,9 +84400,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7361BEC-8853-4EB2-A2A5-7A6BE23ACDAF}">
   <dimension ref="A1:AH49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -88272,9 +88291,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989DF7F6-FD9D-4F5D-98BD-4C3E13B479E3}">
   <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>